<commit_message>
Updated model selection, fixed prior
</commit_message>
<xml_diff>
--- a/data/e-mailing_authors_for_data.xlsx
+++ b/data/e-mailing_authors_for_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxlindmark/Desktop/R_STUDIO_PROJECTS/scaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434261C3-3025-A64B-808D-237DB5D7D261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DDD16A-F8FF-7F4F-B0AC-A2000E14F91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10240" yWindow="460" windowWidth="27840" windowHeight="22160" xr2:uid="{B4C08AE0-3A1E-904B-8E17-AE1A12838F3D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="177">
   <si>
     <t>Rate</t>
   </si>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2332,23 +2332,26 @@
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E62" s="9" t="s">
+      <c r="D62" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="F62" s="9" t="s">
-        <v>154</v>
+      <c r="F62" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>161</v>
       </c>
       <c r="H62" s="4"/>
     </row>

</xml_diff>

<commit_message>
update metabolism data with data from author
</commit_message>
<xml_diff>
--- a/data/e-mailing_authors_for_data.xlsx
+++ b/data/e-mailing_authors_for_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxlindmark/Desktop/R_STUDIO_PROJECTS/scaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DDD16A-F8FF-7F4F-B0AC-A2000E14F91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A166798-6A1A-4D4A-92E4-A3FDFE631DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="460" windowWidth="27840" windowHeight="22160" xr2:uid="{B4C08AE0-3A1E-904B-8E17-AE1A12838F3D}"/>
+    <workbookView xWindow="2960" yWindow="480" windowWidth="31400" windowHeight="22160" xr2:uid="{B4C08AE0-3A1E-904B-8E17-AE1A12838F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="177">
   <si>
     <t>Rate</t>
   </si>
@@ -671,7 +671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -709,6 +709,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1024,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F006A5FD-A392-2548-AFD4-3A7558A73F71}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1699,7 +1700,7 @@
       </c>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>1</v>
       </c>
@@ -1720,28 +1721,32 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="11" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="D34" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F34" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="25"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
@@ -1762,7 +1767,7 @@
       </c>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>92</v>
       </c>
@@ -1783,7 +1788,7 @@
       </c>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>92</v>
       </c>
@@ -1801,7 +1806,7 @@
       </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>92</v>
       </c>
@@ -1819,7 +1824,7 @@
       </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>92</v>
       </c>
@@ -1843,7 +1848,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>92</v>
       </c>
@@ -1864,7 +1869,7 @@
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>92</v>
       </c>
@@ -1888,7 +1893,7 @@
       </c>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>92</v>
       </c>
@@ -1912,7 +1917,7 @@
       </c>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>92</v>
       </c>
@@ -1936,7 +1941,7 @@
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>92</v>
       </c>
@@ -1956,7 +1961,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
         <v>92</v>
       </c>
@@ -1976,7 +1981,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>92</v>
       </c>
@@ -1997,7 +2002,7 @@
       </c>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>92</v>
       </c>
@@ -2023,7 +2028,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>92</v>
       </c>

</xml_diff>